<commit_message>
- Generates Game from XML
</commit_message>
<xml_diff>
--- a/ScrumDoku/Product_Backlog.xlsx
+++ b/ScrumDoku/Product_Backlog.xlsx
@@ -220,9 +220,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -260,7 +260,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -332,7 +332,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -506,10 +506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +621,7 @@
         <v>26</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -835,6 +838,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Sprint Backlogs zusammgengeführt -Product Backlog ergänzt
</commit_message>
<xml_diff>
--- a/ScrumDoku/Product_Backlog.xlsx
+++ b/ScrumDoku/Product_Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>StoryID</t>
   </si>
@@ -103,14 +103,14 @@
     <t>teilweise</t>
   </si>
   <si>
-    <t>S</t>
+    <t>Wird ein Schiffsteil ungültig platziert (zu nah an anderem Schiff, ...) wird das Schiffsteil rot angezeigt.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,7 +229,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -242,29 +242,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -287,9 +293,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -327,9 +333,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,9 +367,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -395,9 +402,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -570,34 +578,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="21">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1">
+      <c r="B1" s="13"/>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -620,302 +628,324 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A4" s="7">
+    <row r="4" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="7">
-        <v>5</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="6">
+        <v>5</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A5" s="7">
+    <row r="5" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>6</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A6" s="7">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>1</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>8</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A7" s="7">
+    <row r="7" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="C7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>4</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A8" s="7">
-        <v>5</v>
-      </c>
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="7">
-        <v>5</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="E8" s="6">
+        <v>5</v>
+      </c>
+      <c r="F8" s="6">
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A9" s="11">
+    <row r="9" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="15">
         <v>2</v>
       </c>
-      <c r="E9" s="11">
-        <v>5</v>
-      </c>
-      <c r="F9" s="11">
+      <c r="E9" s="15">
+        <v>5</v>
+      </c>
+      <c r="F9" s="15">
         <v>2</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>2</v>
+      </c>
+      <c r="E10" s="8">
+        <v>7</v>
+      </c>
+      <c r="F10" s="8">
+        <v>2</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A10" s="9">
+    <row r="11" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8">
+        <v>3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>3</v>
+      </c>
+      <c r="F11" s="8">
+        <v>3</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="15">
+        <v>3</v>
+      </c>
+      <c r="E12" s="15">
         <v>4</v>
       </c>
-      <c r="D10" s="9">
+      <c r="F12" s="15">
+        <v>3</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="15">
+        <v>3</v>
+      </c>
+      <c r="E13" s="15">
+        <v>4</v>
+      </c>
+      <c r="F13" s="15">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8">
+        <v>3</v>
+      </c>
+      <c r="E14" s="8">
+        <v>4</v>
+      </c>
+      <c r="F14" s="8">
         <v>2</v>
       </c>
-      <c r="E10" s="9">
-        <v>7</v>
-      </c>
-      <c r="F10" s="9">
-        <v>2</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="G14" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A11" s="9">
+    <row r="15" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>12</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="10">
+        <v>3</v>
+      </c>
+      <c r="E15" s="10">
+        <v>6</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="9">
-        <v>3</v>
-      </c>
-      <c r="E11" s="9">
-        <v>3</v>
-      </c>
-      <c r="F11" s="9">
-        <v>3</v>
-      </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A12" s="9">
-        <v>9</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="9">
-        <v>3</v>
-      </c>
-      <c r="E12" s="9">
+      <c r="C16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="10">
         <v>4</v>
       </c>
-      <c r="F12" s="9">
-        <v>3</v>
-      </c>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A13" s="9">
-        <v>10</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="9">
-        <v>3</v>
-      </c>
-      <c r="E13" s="9">
-        <v>4</v>
-      </c>
-      <c r="F13" s="9">
-        <v>2</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A14" s="11">
-        <v>11</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="11" t="s">
+      <c r="E16" s="10">
+        <v>3</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
         <v>14</v>
       </c>
-      <c r="D14" s="11">
-        <v>3</v>
-      </c>
-      <c r="E14" s="11">
-        <v>6</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A15" s="11">
-        <v>12</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="11">
-        <v>4</v>
-      </c>
-      <c r="E15" s="11">
-        <v>3</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A16" s="11">
-        <v>13</v>
-      </c>
-      <c r="B16" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="11">
-        <v>5</v>
-      </c>
-      <c r="E16" s="11">
-        <v>5</v>
-      </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" ht="33.75" customHeight="1"/>
-    <row r="18" ht="33.75" customHeight="1"/>
-    <row r="19" ht="33.75" customHeight="1"/>
-    <row r="20" ht="33.75" customHeight="1"/>
-    <row r="21" ht="33.75" customHeight="1"/>
-    <row r="22" ht="33.75" customHeight="1"/>
-    <row r="23" ht="33.75" customHeight="1"/>
-    <row r="24" ht="33.75" customHeight="1"/>
-    <row r="25" ht="33.75" customHeight="1"/>
-    <row r="26" ht="33.75" customHeight="1"/>
+      <c r="D17" s="10">
+        <v>5</v>
+      </c>
+      <c r="E17" s="10">
+        <v>5</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="C4:E15">
     <sortCondition ref="D4:D15"/>

</xml_diff>